<commit_message>
add up transformer and regularization.
</commit_message>
<xml_diff>
--- a/df_Merge_ASDnVehiclenCompany.xlsx
+++ b/df_Merge_ASDnVehiclenCompany.xlsx
@@ -3291,7 +3291,7 @@
         <v>8757</v>
       </c>
       <c r="BQ2">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="BR2">
         <v>497</v>
@@ -3503,7 +3503,7 @@
         <v>4973</v>
       </c>
       <c r="BQ3">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="BR3">
         <v>450</v>
@@ -3927,7 +3927,7 @@
         <v>0</v>
       </c>
       <c r="BQ5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BR5">
         <v>216</v>
@@ -4139,7 +4139,7 @@
         <v>0</v>
       </c>
       <c r="BQ6">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="BR6">
         <v>920</v>
@@ -4351,7 +4351,7 @@
         <v>11079</v>
       </c>
       <c r="BQ7">
-        <v>49</v>
+        <v>100</v>
       </c>
       <c r="BR7">
         <v>1596</v>
@@ -4563,7 +4563,7 @@
         <v>5097</v>
       </c>
       <c r="BQ8">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="BR8">
         <v>399</v>
@@ -4775,7 +4775,7 @@
         <v>0</v>
       </c>
       <c r="BQ9">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="BR9">
         <v>527</v>
@@ -6895,7 +6895,7 @@
         <v>0</v>
       </c>
       <c r="BQ19">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="BR19">
         <v>115</v>
@@ -7107,7 +7107,7 @@
         <v>3856</v>
       </c>
       <c r="BQ20">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="BR20">
         <v>1134</v>
@@ -7955,7 +7955,7 @@
         <v>2242</v>
       </c>
       <c r="BQ24">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="BR24">
         <v>215</v>
@@ -8167,7 +8167,7 @@
         <v>8597</v>
       </c>
       <c r="BQ25">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="BR25">
         <v>240</v>
@@ -8591,7 +8591,7 @@
         <v>4807</v>
       </c>
       <c r="BQ27">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="BR27">
         <v>870</v>
@@ -9439,7 +9439,7 @@
         <v>0</v>
       </c>
       <c r="BQ31">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="BR31">
         <v>896</v>
@@ -9651,7 +9651,7 @@
         <v>0</v>
       </c>
       <c r="BQ32">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="BR32">
         <v>1121</v>
@@ -9863,7 +9863,7 @@
         <v>0</v>
       </c>
       <c r="BQ33">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="BR33">
         <v>788</v>
@@ -10075,7 +10075,7 @@
         <v>0</v>
       </c>
       <c r="BQ34">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="BR34">
         <v>1004</v>
@@ -10499,7 +10499,7 @@
         <v>0</v>
       </c>
       <c r="BQ36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BR36">
         <v>418</v>
@@ -10711,7 +10711,7 @@
         <v>0</v>
       </c>
       <c r="BQ37">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="BR37">
         <v>1351</v>
@@ -10923,7 +10923,7 @@
         <v>0</v>
       </c>
       <c r="BQ38">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="BR38">
         <v>1240</v>
@@ -11135,7 +11135,7 @@
         <v>0</v>
       </c>
       <c r="BQ39">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="BR39">
         <v>1838</v>
@@ -11347,7 +11347,7 @@
         <v>0</v>
       </c>
       <c r="BQ40">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="BR40">
         <v>932</v>
@@ -11559,7 +11559,7 @@
         <v>0</v>
       </c>
       <c r="BQ41">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="BR41">
         <v>1131</v>
@@ -11771,7 +11771,7 @@
         <v>0</v>
       </c>
       <c r="BQ42">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="BR42">
         <v>992</v>
@@ -11983,7 +11983,7 @@
         <v>0</v>
       </c>
       <c r="BQ43">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="BR43">
         <v>1388</v>
@@ -12407,7 +12407,7 @@
         <v>0</v>
       </c>
       <c r="BQ45">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BR45">
         <v>803</v>
@@ -12619,7 +12619,7 @@
         <v>0</v>
       </c>
       <c r="BQ46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BR46">
         <v>145</v>
@@ -12831,7 +12831,7 @@
         <v>0</v>
       </c>
       <c r="BQ47">
-        <v>82</v>
+        <v>206</v>
       </c>
       <c r="BR47">
         <v>1576</v>
@@ -13043,7 +13043,7 @@
         <v>0</v>
       </c>
       <c r="BQ48">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="BR48">
         <v>1703</v>
@@ -13255,7 +13255,7 @@
         <v>0</v>
       </c>
       <c r="BQ49">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="BR49">
         <v>1057</v>
@@ -13467,7 +13467,7 @@
         <v>0</v>
       </c>
       <c r="BQ50">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="BR50">
         <v>1913</v>
@@ -13679,7 +13679,7 @@
         <v>0</v>
       </c>
       <c r="BQ51">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="BR51">
         <v>1195</v>
@@ -13891,7 +13891,7 @@
         <v>0</v>
       </c>
       <c r="BQ52">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="BR52">
         <v>540</v>
@@ -14103,7 +14103,7 @@
         <v>0</v>
       </c>
       <c r="BQ53">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="BR53">
         <v>1654</v>
@@ -14527,7 +14527,7 @@
         <v>0</v>
       </c>
       <c r="BQ55">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="BR55">
         <v>284</v>
@@ -14739,7 +14739,7 @@
         <v>0</v>
       </c>
       <c r="BQ56">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="BR56">
         <v>938</v>
@@ -15587,7 +15587,7 @@
         <v>0</v>
       </c>
       <c r="BQ60">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="BR60">
         <v>959</v>
@@ -15799,7 +15799,7 @@
         <v>0</v>
       </c>
       <c r="BQ61">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="BR61">
         <v>1084</v>
@@ -16223,7 +16223,7 @@
         <v>0</v>
       </c>
       <c r="BQ63">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="BR63">
         <v>578</v>
@@ -16435,7 +16435,7 @@
         <v>0</v>
       </c>
       <c r="BQ64">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="BR64">
         <v>580</v>
@@ -16647,7 +16647,7 @@
         <v>0</v>
       </c>
       <c r="BQ65">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="BR65">
         <v>508</v>
@@ -17071,7 +17071,7 @@
         <v>0</v>
       </c>
       <c r="BQ67">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="BR67">
         <v>1806</v>
@@ -17283,7 +17283,7 @@
         <v>0</v>
       </c>
       <c r="BQ68">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="BR68">
         <v>1059</v>
@@ -17495,7 +17495,7 @@
         <v>0</v>
       </c>
       <c r="BQ69">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="BR69">
         <v>2363</v>
@@ -17707,7 +17707,7 @@
         <v>0</v>
       </c>
       <c r="BQ70">
-        <v>22</v>
+        <v>79</v>
       </c>
       <c r="BR70">
         <v>1067</v>
@@ -17919,7 +17919,7 @@
         <v>0</v>
       </c>
       <c r="BQ71">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="BR71">
         <v>1173</v>
@@ -18343,7 +18343,7 @@
         <v>0</v>
       </c>
       <c r="BQ73">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="BR73">
         <v>1154</v>
@@ -18767,7 +18767,7 @@
         <v>0</v>
       </c>
       <c r="BQ75">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="BR75">
         <v>1498</v>
@@ -19191,7 +19191,7 @@
         <v>0</v>
       </c>
       <c r="BQ77">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="BR77">
         <v>1325</v>
@@ -19827,7 +19827,7 @@
         <v>1650</v>
       </c>
       <c r="BQ80">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="BR80">
         <v>712</v>
@@ -20039,7 +20039,7 @@
         <v>0</v>
       </c>
       <c r="BQ81">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="BR81">
         <v>659</v>
@@ -20251,7 +20251,7 @@
         <v>6617</v>
       </c>
       <c r="BQ82">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="BR82">
         <v>1566</v>
@@ -21311,7 +21311,7 @@
         <v>24617</v>
       </c>
       <c r="BQ87">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="BR87">
         <v>1577</v>
@@ -21523,7 +21523,7 @@
         <v>0</v>
       </c>
       <c r="BQ88">
-        <v>88</v>
+        <v>151</v>
       </c>
       <c r="BR88">
         <v>1491</v>
@@ -21735,7 +21735,7 @@
         <v>34793</v>
       </c>
       <c r="BQ89">
-        <v>55</v>
+        <v>120</v>
       </c>
       <c r="BR89">
         <v>1873</v>
@@ -21947,7 +21947,7 @@
         <v>0</v>
       </c>
       <c r="BQ90">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="BR90">
         <v>1038</v>
@@ -22159,7 +22159,7 @@
         <v>4907</v>
       </c>
       <c r="BQ91">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="BR91">
         <v>702</v>
@@ -22371,7 +22371,7 @@
         <v>33659</v>
       </c>
       <c r="BQ92">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="BR92">
         <v>847</v>
@@ -22583,7 +22583,7 @@
         <v>52513</v>
       </c>
       <c r="BQ93">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="BR93">
         <v>2083</v>
@@ -22795,7 +22795,7 @@
         <v>42836</v>
       </c>
       <c r="BQ94">
-        <v>37</v>
+        <v>93</v>
       </c>
       <c r="BR94">
         <v>1659</v>
@@ -23007,7 +23007,7 @@
         <v>21490</v>
       </c>
       <c r="BQ95">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="BR95">
         <v>1089</v>
@@ -23219,7 +23219,7 @@
         <v>11171</v>
       </c>
       <c r="BQ96">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="BR96">
         <v>962</v>
@@ -23431,7 +23431,7 @@
         <v>19813</v>
       </c>
       <c r="BQ97">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="BR97">
         <v>1276</v>
@@ -23643,7 +23643,7 @@
         <v>3186</v>
       </c>
       <c r="BQ98">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="BR98">
         <v>830</v>
@@ -24491,7 +24491,7 @@
         <v>34643</v>
       </c>
       <c r="BQ102">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="BR102">
         <v>875</v>
@@ -24915,7 +24915,7 @@
         <v>20537</v>
       </c>
       <c r="BQ104">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="BR104">
         <v>462</v>
@@ -25127,7 +25127,7 @@
         <v>17343</v>
       </c>
       <c r="BQ105">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="BR105">
         <v>945</v>
@@ -25339,7 +25339,7 @@
         <v>11444</v>
       </c>
       <c r="BQ106">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="BR106">
         <v>468</v>
@@ -25551,7 +25551,7 @@
         <v>25159</v>
       </c>
       <c r="BQ107">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="BR107">
         <v>622</v>
@@ -25763,7 +25763,7 @@
         <v>33797</v>
       </c>
       <c r="BQ108">
-        <v>57</v>
+        <v>123</v>
       </c>
       <c r="BR108">
         <v>2583</v>
@@ -25975,7 +25975,7 @@
         <v>41150</v>
       </c>
       <c r="BQ109">
-        <v>219</v>
+        <v>245</v>
       </c>
       <c r="BR109">
         <v>1565</v>
@@ -26187,7 +26187,7 @@
         <v>11414</v>
       </c>
       <c r="BQ110">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="BR110">
         <v>687</v>
@@ -26399,7 +26399,7 @@
         <v>19585</v>
       </c>
       <c r="BQ111">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="BR111">
         <v>835</v>
@@ -26611,7 +26611,7 @@
         <v>8719</v>
       </c>
       <c r="BQ112">
-        <v>3</v>
+        <v>63</v>
       </c>
       <c r="BR112">
         <v>245</v>
@@ -26823,7 +26823,7 @@
         <v>20919</v>
       </c>
       <c r="BQ113">
-        <v>23</v>
+        <v>85</v>
       </c>
       <c r="BR113">
         <v>715</v>
@@ -27035,7 +27035,7 @@
         <v>10142</v>
       </c>
       <c r="BQ114">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="BR114">
         <v>504</v>
@@ -27247,7 +27247,7 @@
         <v>18219</v>
       </c>
       <c r="BQ115">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="BR115">
         <v>591</v>
@@ -27459,7 +27459,7 @@
         <v>30376</v>
       </c>
       <c r="BQ116">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="BR116">
         <v>1793</v>
@@ -27671,7 +27671,7 @@
         <v>14743</v>
       </c>
       <c r="BQ117">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="BR117">
         <v>1270</v>
@@ -27883,7 +27883,7 @@
         <v>27389</v>
       </c>
       <c r="BQ118">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="BR118">
         <v>540</v>
@@ -28095,7 +28095,7 @@
         <v>33884</v>
       </c>
       <c r="BQ119">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="BR119">
         <v>756</v>
@@ -28519,7 +28519,7 @@
         <v>28499</v>
       </c>
       <c r="BQ121">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="BR121">
         <v>2579</v>
@@ -28731,7 +28731,7 @@
         <v>21063</v>
       </c>
       <c r="BQ122">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="BR122">
         <v>948</v>
@@ -28943,7 +28943,7 @@
         <v>18531</v>
       </c>
       <c r="BQ123">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="BR123">
         <v>1730</v>
@@ -29155,7 +29155,7 @@
         <v>33310</v>
       </c>
       <c r="BQ124">
-        <v>40</v>
+        <v>92</v>
       </c>
       <c r="BR124">
         <v>1135</v>
@@ -29367,7 +29367,7 @@
         <v>8304</v>
       </c>
       <c r="BQ125">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="BR125">
         <v>1034</v>
@@ -30003,7 +30003,7 @@
         <v>0</v>
       </c>
       <c r="BQ128">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BR128">
         <v>90</v>
@@ -30639,7 +30639,7 @@
         <v>5648</v>
       </c>
       <c r="BQ131">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="BR131">
         <v>1188</v>
@@ -30851,7 +30851,7 @@
         <v>14268</v>
       </c>
       <c r="BQ132">
-        <v>31</v>
+        <v>86</v>
       </c>
       <c r="BR132">
         <v>1118</v>
@@ -31063,7 +31063,7 @@
         <v>14317</v>
       </c>
       <c r="BQ133">
-        <v>48</v>
+        <v>96</v>
       </c>
       <c r="BR133">
         <v>2231</v>
@@ -31275,7 +31275,7 @@
         <v>23791</v>
       </c>
       <c r="BQ134">
-        <v>369</v>
+        <v>552</v>
       </c>
       <c r="BR134">
         <v>3544</v>
@@ -31487,7 +31487,7 @@
         <v>9912</v>
       </c>
       <c r="BQ135">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BR135">
         <v>368</v>
@@ -31699,7 +31699,7 @@
         <v>4586</v>
       </c>
       <c r="BQ136">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="BR136">
         <v>1215</v>
@@ -31911,7 +31911,7 @@
         <v>4205</v>
       </c>
       <c r="BQ137">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BR137">
         <v>781</v>
@@ -32123,7 +32123,7 @@
         <v>12217</v>
       </c>
       <c r="BQ138">
-        <v>23</v>
+        <v>357</v>
       </c>
       <c r="BR138">
         <v>1112</v>
@@ -32335,7 +32335,7 @@
         <v>16701</v>
       </c>
       <c r="BQ139">
-        <v>62</v>
+        <v>465</v>
       </c>
       <c r="BR139">
         <v>2466</v>
@@ -32547,7 +32547,7 @@
         <v>14726</v>
       </c>
       <c r="BQ140">
-        <v>60</v>
+        <v>109</v>
       </c>
       <c r="BR140">
         <v>1440</v>
@@ -32971,7 +32971,7 @@
         <v>6325</v>
       </c>
       <c r="BQ142">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BR142">
         <v>448</v>
@@ -35727,7 +35727,7 @@
         <v>7553</v>
       </c>
       <c r="BQ155">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="BR155">
         <v>1811</v>
@@ -35939,7 +35939,7 @@
         <v>1571</v>
       </c>
       <c r="BQ156">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="BR156">
         <v>888</v>
@@ -36151,7 +36151,7 @@
         <v>4034</v>
       </c>
       <c r="BQ157">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="BR157">
         <v>1758</v>
@@ -36363,7 +36363,7 @@
         <v>2287</v>
       </c>
       <c r="BQ158">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="BR158">
         <v>1230</v>
@@ -36575,7 +36575,7 @@
         <v>2876</v>
       </c>
       <c r="BQ159">
-        <v>191</v>
+        <v>225</v>
       </c>
       <c r="BR159">
         <v>972</v>
@@ -37423,7 +37423,7 @@
         <v>900</v>
       </c>
       <c r="BQ163">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="BR163">
         <v>637</v>
@@ -37635,7 +37635,7 @@
         <v>10472</v>
       </c>
       <c r="BQ164">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="BR164">
         <v>926</v>
@@ -37847,7 +37847,7 @@
         <v>9521</v>
       </c>
       <c r="BQ165">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="BR165">
         <v>1142</v>
@@ -38059,7 +38059,7 @@
         <v>6117</v>
       </c>
       <c r="BQ166">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="BR166">
         <v>1007</v>
@@ -38271,7 +38271,7 @@
         <v>2202</v>
       </c>
       <c r="BQ167">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="BR167">
         <v>703</v>
@@ -38483,7 +38483,7 @@
         <v>1028</v>
       </c>
       <c r="BQ168">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="BR168">
         <v>765</v>
@@ -38907,7 +38907,7 @@
         <v>7779</v>
       </c>
       <c r="BQ170">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="BR170">
         <v>1025</v>
@@ -39543,7 +39543,7 @@
         <v>0</v>
       </c>
       <c r="BQ173">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="BR173">
         <v>422</v>
@@ -39755,7 +39755,7 @@
         <v>1756</v>
       </c>
       <c r="BQ174">
-        <v>96</v>
+        <v>181</v>
       </c>
       <c r="BR174">
         <v>2198</v>
@@ -39967,7 +39967,7 @@
         <v>2534</v>
       </c>
       <c r="BQ175">
-        <v>75</v>
+        <v>269</v>
       </c>
       <c r="BR175">
         <v>1532</v>
@@ -40391,7 +40391,7 @@
         <v>2412</v>
       </c>
       <c r="BQ177">
-        <v>68</v>
+        <v>168</v>
       </c>
       <c r="BR177">
         <v>2759</v>
@@ -40603,7 +40603,7 @@
         <v>4222</v>
       </c>
       <c r="BQ178">
-        <v>100</v>
+        <v>164</v>
       </c>
       <c r="BR178">
         <v>1993</v>
@@ -40815,7 +40815,7 @@
         <v>1033</v>
       </c>
       <c r="BQ179">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BR179">
         <v>292</v>
@@ -41027,7 +41027,7 @@
         <v>3775</v>
       </c>
       <c r="BQ180">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="BR180">
         <v>2069</v>
@@ -41451,7 +41451,7 @@
         <v>9808</v>
       </c>
       <c r="BQ182">
-        <v>72</v>
+        <v>149</v>
       </c>
       <c r="BR182">
         <v>1238</v>
@@ -41663,7 +41663,7 @@
         <v>10894</v>
       </c>
       <c r="BQ183">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="BR183">
         <v>1056</v>
@@ -41875,7 +41875,7 @@
         <v>7971</v>
       </c>
       <c r="BQ184">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="BR184">
         <v>804</v>
@@ -42087,7 +42087,7 @@
         <v>2491</v>
       </c>
       <c r="BQ185">
-        <v>52</v>
+        <v>131</v>
       </c>
       <c r="BR185">
         <v>1418</v>
@@ -42723,7 +42723,7 @@
         <v>0</v>
       </c>
       <c r="BQ188">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BR188">
         <v>111</v>
@@ -42935,7 +42935,7 @@
         <v>0</v>
       </c>
       <c r="BQ189">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BR189">
         <v>217</v>
@@ -43571,7 +43571,7 @@
         <v>5288</v>
       </c>
       <c r="BQ192">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="BR192">
         <v>1489</v>
@@ -43995,7 +43995,7 @@
         <v>0</v>
       </c>
       <c r="BQ194">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="BR194">
         <v>977</v>
@@ -44207,7 +44207,7 @@
         <v>0</v>
       </c>
       <c r="BQ195">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BR195">
         <v>869</v>
@@ -44419,7 +44419,7 @@
         <v>7585</v>
       </c>
       <c r="BQ196">
-        <v>10</v>
+        <v>88</v>
       </c>
       <c r="BR196">
         <v>1572</v>
@@ -44631,7 +44631,7 @@
         <v>1698</v>
       </c>
       <c r="BQ197">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="BR197">
         <v>525</v>
@@ -45691,7 +45691,7 @@
         <v>3765</v>
       </c>
       <c r="BQ202">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="BR202">
         <v>716</v>
@@ -45903,7 +45903,7 @@
         <v>3197</v>
       </c>
       <c r="BQ203">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="BR203">
         <v>1024</v>
@@ -46115,7 +46115,7 @@
         <v>1547</v>
       </c>
       <c r="BQ204">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="BR204">
         <v>489</v>
@@ -46327,7 +46327,7 @@
         <v>0</v>
       </c>
       <c r="BQ205">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BR205">
         <v>292</v>
@@ -46539,7 +46539,7 @@
         <v>0</v>
       </c>
       <c r="BQ206">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="BR206">
         <v>837</v>
@@ -47387,7 +47387,7 @@
         <v>4075</v>
       </c>
       <c r="BQ210">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="BR210">
         <v>547</v>
@@ -47599,7 +47599,7 @@
         <v>10028</v>
       </c>
       <c r="BQ211">
-        <v>84</v>
+        <v>117</v>
       </c>
       <c r="BR211">
         <v>1137</v>
@@ -47811,7 +47811,7 @@
         <v>0</v>
       </c>
       <c r="BQ212">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="BR212">
         <v>836</v>
@@ -48235,7 +48235,7 @@
         <v>0</v>
       </c>
       <c r="BQ214">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="BR214">
         <v>890</v>
@@ -48447,7 +48447,7 @@
         <v>7075</v>
       </c>
       <c r="BQ215">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="BR215">
         <v>1297</v>
@@ -48659,7 +48659,7 @@
         <v>14890</v>
       </c>
       <c r="BQ216">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="BR216">
         <v>980</v>
@@ -48871,7 +48871,7 @@
         <v>0</v>
       </c>
       <c r="BQ217">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BR217">
         <v>491</v>
@@ -49083,7 +49083,7 @@
         <v>4336</v>
       </c>
       <c r="BQ218">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="BR218">
         <v>1279</v>
@@ -49295,7 +49295,7 @@
         <v>6654</v>
       </c>
       <c r="BQ219">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="BR219">
         <v>620</v>
@@ -49507,7 +49507,7 @@
         <v>10765</v>
       </c>
       <c r="BQ220">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="BR220">
         <v>830</v>
@@ -49719,7 +49719,7 @@
         <v>0</v>
       </c>
       <c r="BQ221">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="BR221">
         <v>1225</v>
@@ -49931,7 +49931,7 @@
         <v>8341</v>
       </c>
       <c r="BQ222">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="BR222">
         <v>1177</v>
@@ -50143,7 +50143,7 @@
         <v>0</v>
       </c>
       <c r="BQ223">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="BR223">
         <v>476</v>
@@ -50567,7 +50567,7 @@
         <v>0</v>
       </c>
       <c r="BQ225">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="BR225">
         <v>390</v>
@@ -50779,7 +50779,7 @@
         <v>0</v>
       </c>
       <c r="BQ226">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="BR226">
         <v>450</v>
@@ -50991,7 +50991,7 @@
         <v>8680</v>
       </c>
       <c r="BQ227">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="BR227">
         <v>588</v>
@@ -51415,7 +51415,7 @@
         <v>5552</v>
       </c>
       <c r="BQ229">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="BR229">
         <v>401</v>
@@ -51627,7 +51627,7 @@
         <v>7009</v>
       </c>
       <c r="BQ230">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="BR230">
         <v>787</v>
@@ -51839,7 +51839,7 @@
         <v>2047</v>
       </c>
       <c r="BQ231">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BR231">
         <v>331</v>
@@ -52051,7 +52051,7 @@
         <v>2386</v>
       </c>
       <c r="BQ232">
-        <v>55</v>
+        <v>154</v>
       </c>
       <c r="BR232">
         <v>1627</v>
@@ -52263,7 +52263,7 @@
         <v>0</v>
       </c>
       <c r="BQ233">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="BR233">
         <v>1059</v>
@@ -52899,7 +52899,7 @@
         <v>1802</v>
       </c>
       <c r="BQ236">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="BR236">
         <v>806</v>
@@ -53323,7 +53323,7 @@
         <v>654</v>
       </c>
       <c r="BQ238">
-        <v>69</v>
+        <v>307</v>
       </c>
       <c r="BR238">
         <v>1717</v>
@@ -53747,7 +53747,7 @@
         <v>2642</v>
       </c>
       <c r="BQ240">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="BR240">
         <v>798</v>
@@ -53959,7 +53959,7 @@
         <v>2636</v>
       </c>
       <c r="BQ241">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="BR241">
         <v>1764</v>
@@ -54171,7 +54171,7 @@
         <v>0</v>
       </c>
       <c r="BQ242">
-        <v>38</v>
+        <v>96</v>
       </c>
       <c r="BR242">
         <v>2163</v>
@@ -54807,7 +54807,7 @@
         <v>0</v>
       </c>
       <c r="BQ245">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="BR245">
         <v>1134</v>
@@ -55019,7 +55019,7 @@
         <v>0</v>
       </c>
       <c r="BQ246">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="BR246">
         <v>382</v>
@@ -55655,7 +55655,7 @@
         <v>0</v>
       </c>
       <c r="BQ249">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="BR249">
         <v>1402</v>
@@ -56079,7 +56079,7 @@
         <v>0</v>
       </c>
       <c r="BQ251">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="BR251">
         <v>1780</v>
@@ -56291,7 +56291,7 @@
         <v>0</v>
       </c>
       <c r="BQ252">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="BR252">
         <v>2834</v>
@@ -56503,7 +56503,7 @@
         <v>0</v>
       </c>
       <c r="BQ253">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="BR253">
         <v>2643</v>
@@ -56927,7 +56927,7 @@
         <v>1286</v>
       </c>
       <c r="BQ255">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="BR255">
         <v>2399</v>
@@ -57139,7 +57139,7 @@
         <v>6081</v>
       </c>
       <c r="BQ256">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="BR256">
         <v>2092</v>
@@ -57351,7 +57351,7 @@
         <v>0</v>
       </c>
       <c r="BQ257">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="BR257">
         <v>1898</v>
@@ -58199,7 +58199,7 @@
         <v>0</v>
       </c>
       <c r="BQ261">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="BR261">
         <v>1395</v>
@@ -58411,7 +58411,7 @@
         <v>0</v>
       </c>
       <c r="BQ262">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="BR262">
         <v>1912</v>
@@ -58623,7 +58623,7 @@
         <v>0</v>
       </c>
       <c r="BQ263">
-        <v>109</v>
+        <v>131</v>
       </c>
       <c r="BR263">
         <v>1872</v>
@@ -58835,7 +58835,7 @@
         <v>1892</v>
       </c>
       <c r="BQ264">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="BR264">
         <v>1248</v>
@@ -59259,7 +59259,7 @@
         <v>0</v>
       </c>
       <c r="BQ266">
-        <v>99</v>
+        <v>301</v>
       </c>
       <c r="BR266">
         <v>2234</v>
@@ -59471,7 +59471,7 @@
         <v>842</v>
       </c>
       <c r="BQ267">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="BR267">
         <v>823</v>
@@ -59683,7 +59683,7 @@
         <v>0</v>
       </c>
       <c r="BQ268">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="BR268">
         <v>184</v>
@@ -60531,7 +60531,7 @@
         <v>9446</v>
       </c>
       <c r="BQ272">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="BR272">
         <v>833</v>
@@ -60743,7 +60743,7 @@
         <v>3114</v>
       </c>
       <c r="BQ273">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="BR273">
         <v>1413</v>
@@ -60955,7 +60955,7 @@
         <v>2795</v>
       </c>
       <c r="BQ274">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="BR274">
         <v>585</v>
@@ -61167,7 +61167,7 @@
         <v>1156</v>
       </c>
       <c r="BQ275">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="BR275">
         <v>889</v>
@@ -61379,7 +61379,7 @@
         <v>0</v>
       </c>
       <c r="BQ276">
-        <v>40</v>
+        <v>114</v>
       </c>
       <c r="BR276">
         <v>1469</v>
@@ -62227,7 +62227,7 @@
         <v>643</v>
       </c>
       <c r="BQ280">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="BR280">
         <v>423</v>
@@ -62439,7 +62439,7 @@
         <v>0</v>
       </c>
       <c r="BQ281">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="BR281">
         <v>283</v>
@@ -62863,7 +62863,7 @@
         <v>0</v>
       </c>
       <c r="BQ283">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="BR283">
         <v>327</v>
@@ -63075,7 +63075,7 @@
         <v>0</v>
       </c>
       <c r="BQ284">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BR284">
         <v>545</v>
@@ -63499,7 +63499,7 @@
         <v>5355</v>
       </c>
       <c r="BQ286">
-        <v>59</v>
+        <v>115</v>
       </c>
       <c r="BR286">
         <v>2576</v>
@@ -63711,7 +63711,7 @@
         <v>1876</v>
       </c>
       <c r="BQ287">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BR287">
         <v>466</v>
@@ -64347,7 +64347,7 @@
         <v>5352</v>
       </c>
       <c r="BQ290">
-        <v>127</v>
+        <v>272</v>
       </c>
       <c r="BR290">
         <v>1169</v>
@@ -64771,7 +64771,7 @@
         <v>0</v>
       </c>
       <c r="BQ292">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="BR292">
         <v>957</v>
@@ -65831,7 +65831,7 @@
         <v>0</v>
       </c>
       <c r="BQ297">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BR297">
         <v>620</v>
@@ -66043,7 +66043,7 @@
         <v>0</v>
       </c>
       <c r="BQ298">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="BR298">
         <v>756</v>
@@ -66255,7 +66255,7 @@
         <v>0</v>
       </c>
       <c r="BQ299">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="BR299">
         <v>699</v>
@@ -66891,7 +66891,7 @@
         <v>8349</v>
       </c>
       <c r="BQ302">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="BR302">
         <v>748</v>
@@ -67103,7 +67103,7 @@
         <v>7115</v>
       </c>
       <c r="BQ303">
-        <v>75</v>
+        <v>194</v>
       </c>
       <c r="BR303">
         <v>890</v>
@@ -67315,7 +67315,7 @@
         <v>0</v>
       </c>
       <c r="BQ304">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="BR304">
         <v>1085</v>
@@ -68375,7 +68375,7 @@
         <v>0</v>
       </c>
       <c r="BQ309">
-        <v>67</v>
+        <v>317</v>
       </c>
       <c r="BR309">
         <v>1250</v>
@@ -68587,7 +68587,7 @@
         <v>4090</v>
       </c>
       <c r="BQ310">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="BR310">
         <v>1378</v>
@@ -68799,7 +68799,7 @@
         <v>4124</v>
       </c>
       <c r="BQ311">
-        <v>64</v>
+        <v>150</v>
       </c>
       <c r="BR311">
         <v>1736</v>
@@ -69011,7 +69011,7 @@
         <v>0</v>
       </c>
       <c r="BQ312">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="BR312">
         <v>724</v>
@@ -69223,7 +69223,7 @@
         <v>0</v>
       </c>
       <c r="BQ313">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="BR313">
         <v>595</v>
@@ -69647,7 +69647,7 @@
         <v>1319</v>
       </c>
       <c r="BQ315">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="BR315">
         <v>3139</v>
@@ -69859,7 +69859,7 @@
         <v>0</v>
       </c>
       <c r="BQ316">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="BR316">
         <v>1382</v>
@@ -70071,7 +70071,7 @@
         <v>4414</v>
       </c>
       <c r="BQ317">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="BR317">
         <v>1627</v>
@@ -70283,7 +70283,7 @@
         <v>0</v>
       </c>
       <c r="BQ318">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BR318">
         <v>1267</v>
@@ -70495,7 +70495,7 @@
         <v>2334</v>
       </c>
       <c r="BQ319">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BR319">
         <v>218</v>
@@ -70707,7 +70707,7 @@
         <v>4463</v>
       </c>
       <c r="BQ320">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="BR320">
         <v>322</v>
@@ -71131,7 +71131,7 @@
         <v>5435</v>
       </c>
       <c r="BQ322">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="BR322">
         <v>319</v>
@@ -71767,7 +71767,7 @@
         <v>0</v>
       </c>
       <c r="BQ325">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BR325">
         <v>995</v>
@@ -72403,7 +72403,7 @@
         <v>0</v>
       </c>
       <c r="BQ328">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="BR328">
         <v>73</v>
@@ -72827,7 +72827,7 @@
         <v>41297</v>
       </c>
       <c r="BQ330">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BR330">
         <v>356</v>
@@ -73039,7 +73039,7 @@
         <v>60990</v>
       </c>
       <c r="BQ331">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="BR331">
         <v>773</v>
@@ -73251,7 +73251,7 @@
         <v>79120</v>
       </c>
       <c r="BQ332">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="BR332">
         <v>1222</v>
@@ -73463,7 +73463,7 @@
         <v>76169</v>
       </c>
       <c r="BQ333">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="BR333">
         <v>629</v>
@@ -73675,7 +73675,7 @@
         <v>112240</v>
       </c>
       <c r="BQ334">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="BR334">
         <v>752</v>
@@ -73887,7 +73887,7 @@
         <v>53158</v>
       </c>
       <c r="BQ335">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="BR335">
         <v>468</v>
@@ -74523,7 +74523,7 @@
         <v>113157</v>
       </c>
       <c r="BQ338">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="BR338">
         <v>1277</v>
@@ -74735,7 +74735,7 @@
         <v>88781</v>
       </c>
       <c r="BQ339">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="BR339">
         <v>1025</v>
@@ -74947,7 +74947,7 @@
         <v>118854</v>
       </c>
       <c r="BQ340">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="BR340">
         <v>713</v>
@@ -75371,7 +75371,7 @@
         <v>81597</v>
       </c>
       <c r="BQ342">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="BR342">
         <v>764</v>
@@ -75583,7 +75583,7 @@
         <v>162363</v>
       </c>
       <c r="BQ343">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="BR343">
         <v>1236</v>
@@ -76219,7 +76219,7 @@
         <v>256631</v>
       </c>
       <c r="BQ346">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="BR346">
         <v>2562</v>
@@ -76431,7 +76431,7 @@
         <v>196832</v>
       </c>
       <c r="BQ347">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="BR347">
         <v>2094</v>
@@ -76643,7 +76643,7 @@
         <v>183902</v>
       </c>
       <c r="BQ348">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="BR348">
         <v>1443</v>
@@ -76855,7 +76855,7 @@
         <v>0</v>
       </c>
       <c r="BQ349">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="BR349">
         <v>1042</v>
@@ -77067,7 +77067,7 @@
         <v>203776</v>
       </c>
       <c r="BQ350">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="BR350">
         <v>1630</v>
@@ -77279,7 +77279,7 @@
         <v>235686</v>
       </c>
       <c r="BQ351">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="BR351">
         <v>1674</v>
@@ -77915,7 +77915,7 @@
         <v>110279</v>
       </c>
       <c r="BQ354">
-        <v>60</v>
+        <v>125</v>
       </c>
       <c r="BR354">
         <v>2090</v>
@@ -78127,7 +78127,7 @@
         <v>38589</v>
       </c>
       <c r="BQ355">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="BR355">
         <v>938</v>
@@ -78551,7 +78551,7 @@
         <v>3345</v>
       </c>
       <c r="BQ357">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BR357">
         <v>174</v>
@@ -78763,7 +78763,7 @@
         <v>79820</v>
       </c>
       <c r="BQ358">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="BR358">
         <v>1477</v>
@@ -78975,7 +78975,7 @@
         <v>70780</v>
       </c>
       <c r="BQ359">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="BR359">
         <v>942</v>
@@ -79187,7 +79187,7 @@
         <v>76737</v>
       </c>
       <c r="BQ360">
-        <v>88</v>
+        <v>123</v>
       </c>
       <c r="BR360">
         <v>1252</v>
@@ -79399,7 +79399,7 @@
         <v>58537</v>
       </c>
       <c r="BQ361">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BR361">
         <v>910</v>
@@ -79611,7 +79611,7 @@
         <v>7307</v>
       </c>
       <c r="BQ362">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BR362">
         <v>307</v>
@@ -79823,7 +79823,7 @@
         <v>79683</v>
       </c>
       <c r="BQ363">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="BR363">
         <v>1664</v>
@@ -80035,7 +80035,7 @@
         <v>108578</v>
       </c>
       <c r="BQ364">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="BR364">
         <v>1654</v>
@@ -80883,7 +80883,7 @@
         <v>107569</v>
       </c>
       <c r="BQ368">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="BR368">
         <v>741</v>
@@ -81095,7 +81095,7 @@
         <v>79888</v>
       </c>
       <c r="BQ369">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="BR369">
         <v>806</v>
@@ -81307,7 +81307,7 @@
         <v>131596</v>
       </c>
       <c r="BQ370">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="BR370">
         <v>1693</v>
@@ -81519,7 +81519,7 @@
         <v>82977</v>
       </c>
       <c r="BQ371">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="BR371">
         <v>1065</v>
@@ -81731,7 +81731,7 @@
         <v>93722</v>
       </c>
       <c r="BQ372">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="BR372">
         <v>697</v>
@@ -82155,7 +82155,7 @@
         <v>64406</v>
       </c>
       <c r="BQ374">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="BR374">
         <v>565</v>
@@ -82367,7 +82367,7 @@
         <v>93546</v>
       </c>
       <c r="BQ375">
-        <v>42</v>
+        <v>109</v>
       </c>
       <c r="BR375">
         <v>930</v>
@@ -82579,7 +82579,7 @@
         <v>92937</v>
       </c>
       <c r="BQ376">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="BR376">
         <v>1002</v>
@@ -82791,7 +82791,7 @@
         <v>127901</v>
       </c>
       <c r="BQ377">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="BR377">
         <v>1044</v>
@@ -83003,7 +83003,7 @@
         <v>80983</v>
       </c>
       <c r="BQ378">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="BR378">
         <v>628</v>
@@ -83215,7 +83215,7 @@
         <v>0</v>
       </c>
       <c r="BQ379">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BR379">
         <v>174</v>
@@ -83427,7 +83427,7 @@
         <v>0</v>
       </c>
       <c r="BQ380">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="BR380">
         <v>153</v>
@@ -84275,7 +84275,7 @@
         <v>5272</v>
       </c>
       <c r="BQ384">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BR384">
         <v>52</v>
@@ -84699,7 +84699,7 @@
         <v>32027</v>
       </c>
       <c r="BQ386">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="BR386">
         <v>357</v>
@@ -85123,7 +85123,7 @@
         <v>59112</v>
       </c>
       <c r="BQ388">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="BR388">
         <v>760</v>
@@ -85335,7 +85335,7 @@
         <v>61086</v>
       </c>
       <c r="BQ389">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="BR389">
         <v>366</v>
@@ -85547,7 +85547,7 @@
         <v>34796</v>
       </c>
       <c r="BQ390">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="BR390">
         <v>445</v>
@@ -85759,7 +85759,7 @@
         <v>45286</v>
       </c>
       <c r="BQ391">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="BR391">
         <v>578</v>
@@ -85971,7 +85971,7 @@
         <v>51437</v>
       </c>
       <c r="BQ392">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="BR392">
         <v>372</v>
@@ -86607,7 +86607,7 @@
         <v>0</v>
       </c>
       <c r="BQ395">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="BR395">
         <v>479</v>
@@ -87243,7 +87243,7 @@
         <v>34370</v>
       </c>
       <c r="BQ398">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BR398">
         <v>527</v>
@@ -87455,7 +87455,7 @@
         <v>43588</v>
       </c>
       <c r="BQ399">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="BR399">
         <v>611</v>
@@ -87667,7 +87667,7 @@
         <v>35867</v>
       </c>
       <c r="BQ400">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="BR400">
         <v>839</v>
@@ -87879,7 +87879,7 @@
         <v>31573</v>
       </c>
       <c r="BQ401">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="BR401">
         <v>376</v>
@@ -88091,7 +88091,7 @@
         <v>30009</v>
       </c>
       <c r="BQ402">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="BR402">
         <v>1325</v>

</xml_diff>